<commit_message>
Small fixes. IEEE import working. Working on line flows.
</commit_message>
<xml_diff>
--- a/simplepower/models/grid_model_data/grid_data4.xlsx
+++ b/simplepower/models/grid_model_data/grid_data4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/grid_model_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A871536-1227-4F79-B3AA-8E49A0D96209}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C188485-54B8-4C96-AFD1-8F11960A86F7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
   </bookViews>
   <sheets>
     <sheet name="busbars" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>b_shunt_pu</t>
+  </si>
+  <si>
+    <t>v_base_kV</t>
   </si>
 </sst>
 </file>
@@ -220,6 +223,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,14 +532,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -543,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -554,7 +561,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -565,7 +572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -589,16 +596,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -665,16 +672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF97191-B8C8-4B12-8921-F601069D1D4E}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -745,12 +752,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -787,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -807,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -817,19 +824,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C15A9-E0D3-48E6-90F6-6A9120B37C7B}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,37 +850,40 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -887,33 +897,36 @@
         <v>22</v>
       </c>
       <c r="E2">
+        <v>132</v>
+      </c>
+      <c r="F2">
         <v>0.03</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.05</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1E-3</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>0.01</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>-5</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>5</v>
       </c>
     </row>

</xml_diff>